<commit_message>
Second commit tested, rerun, data driven scenarios
</commit_message>
<xml_diff>
--- a/testData/Opencart_LoginData.xlsx
+++ b/testData/Opencart_LoginData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pavan\Aug19Batch\opencart_cucumber_framework\testData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\burha\eclipse-workspace\opencart_cucumber_V1\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{713E5A9A-8C65-466B-BB3D-5AB006CE15A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89A2DD92-3E07-4A3D-9E7A-333207964CFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="17589" xr2:uid="{1F2D179E-37D2-4BC0-88A9-F5C135B87DA5}"/>
+    <workbookView xWindow="3240" yWindow="3045" windowWidth="15375" windowHeight="7875" xr2:uid="{1F2D179E-37D2-4BC0-88A9-F5C135B87DA5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,21 +20,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="15">
   <si>
     <t>username</t>
   </si>
@@ -69,13 +60,16 @@
     <t>xyz</t>
   </si>
   <si>
-    <t>pavanoltraining@gmail.com</t>
-  </si>
-  <si>
-    <t>test@123</t>
-  </si>
-  <si>
-    <t>abc123@gmail.com</t>
+    <t>test@1234</t>
+  </si>
+  <si>
+    <t>rebotraining@gmail.com</t>
+  </si>
+  <si>
+    <t>rebo2@gmail.com</t>
+  </si>
+  <si>
+    <t>Retest@123</t>
   </si>
 </sst>
 </file>
@@ -141,7 +135,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -153,9 +147,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -476,17 +467,17 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.15234375" customWidth="1"/>
-    <col min="2" max="2" width="17.3046875" customWidth="1"/>
-    <col min="3" max="3" width="18.15234375" customWidth="1"/>
+    <col min="1" max="1" width="27.140625" customWidth="1"/>
+    <col min="2" max="2" width="17.28515625" customWidth="1"/>
+    <col min="3" max="3" width="18.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -497,18 +488,18 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>11</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>12</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
@@ -519,7 +510,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
@@ -530,7 +521,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>9</v>
       </c>
@@ -541,26 +532,26 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>13</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="3" t="s">
         <v>5</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{D3BE7519-95C3-4ACD-9AB4-5385C9508082}"/>
-    <hyperlink ref="A4" r:id="rId2" xr:uid="{8456409A-CACC-4B7E-B78E-75E713148E0E}"/>
-    <hyperlink ref="A3" r:id="rId3" xr:uid="{5E52A498-5B14-4BDC-BBF1-05425B8AC197}"/>
-    <hyperlink ref="A5" r:id="rId4" xr:uid="{94E9D5A6-98A1-4A25-BDDE-C5B20EDA887E}"/>
-    <hyperlink ref="B2" r:id="rId5" xr:uid="{968262D0-AE14-41EF-AB8A-08B3F886E797}"/>
-    <hyperlink ref="A6" r:id="rId6" xr:uid="{75A4F8D6-7BF1-446B-9367-475FA4FB44C7}"/>
-    <hyperlink ref="B6" r:id="rId7" xr:uid="{01D5649A-5E55-45E1-9B81-1CE430C208A1}"/>
+    <hyperlink ref="A4" r:id="rId1" xr:uid="{8456409A-CACC-4B7E-B78E-75E713148E0E}"/>
+    <hyperlink ref="A3" r:id="rId2" xr:uid="{5E52A498-5B14-4BDC-BBF1-05425B8AC197}"/>
+    <hyperlink ref="A5" r:id="rId3" xr:uid="{94E9D5A6-98A1-4A25-BDDE-C5B20EDA887E}"/>
+    <hyperlink ref="B2" r:id="rId4" xr:uid="{968262D0-AE14-41EF-AB8A-08B3F886E797}"/>
+    <hyperlink ref="A6" r:id="rId5" xr:uid="{75A4F8D6-7BF1-446B-9367-475FA4FB44C7}"/>
+    <hyperlink ref="B6" r:id="rId6" xr:uid="{01D5649A-5E55-45E1-9B81-1CE430C208A1}"/>
+    <hyperlink ref="A2" r:id="rId7" xr:uid="{D3BE7519-95C3-4ACD-9AB4-5385C9508082}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId8"/>

</xml_diff>